<commit_message>
added option to pre-load only textures
</commit_message>
<xml_diff>
--- a/build files and notes/fluff/sheet w build methods info.xlsx
+++ b/build files and notes/fluff/sheet w build methods info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/fluff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\fluff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="915" documentId="13_ncr:1_{3F0C8CE3-8F4B-444B-8ACA-978327A75101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7114A9C1-F130-492E-86EC-3FB3793E423C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91C5E40-7C8A-407B-BAB9-CE3B5E06CDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="0" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="All level build notes" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="171">
   <si>
     <t>0A</t>
   </si>
@@ -360,9 +360,6 @@
     <t>4, limit 20 mult 1.5 seed 27626, built iter 0</t>
   </si>
   <si>
-    <t>LL regen settings</t>
-  </si>
-  <si>
     <t>Spawn</t>
   </si>
   <si>
@@ -387,12 +384,6 @@
     <t>Iter count, best result</t>
   </si>
   <si>
-    <t>6000/6000/6000/1/0.15</t>
-  </si>
-  <si>
-    <t>5500/5500/5500/1/0.20</t>
-  </si>
-  <si>
     <t>500,   1 - 2020202020201919</t>
   </si>
   <si>
@@ -429,15 +420,9 @@
     <t>01_aZ - 1</t>
   </si>
   <si>
-    <t>6000/6000/6000/1/0.00</t>
-  </si>
-  <si>
     <t>0a_dZ - 2</t>
   </si>
   <si>
-    <t>7000/7000/7000/1/0.00</t>
-  </si>
-  <si>
     <t>4, limit 20, mult 1.5 seed 25579</t>
   </si>
   <si>
@@ -456,9 +441,6 @@
     <t>00_eZ - 1</t>
   </si>
   <si>
-    <t>8000/8000/8000/1/0.00</t>
-  </si>
-  <si>
     <t>4, limit 15, mult 1.5 seed  1749</t>
   </si>
   <si>
@@ -486,9 +468,6 @@
     <t>general wrong 9-38</t>
   </si>
   <si>
-    <t>6000/6000/6000/1/0.20</t>
-  </si>
-  <si>
     <t>4, limit 19, mult 1.5 seed  7989</t>
   </si>
   <si>
@@ -507,9 +486,6 @@
     <t>02_fZ - 1</t>
   </si>
   <si>
-    <t>4000/4000/4000/1/0.00</t>
-  </si>
-  <si>
     <t>Special notes</t>
   </si>
   <si>
@@ -531,19 +507,46 @@
     <t>01_pZ - 1</t>
   </si>
   <si>
-    <t>5500/5500/5500/0/0.00</t>
-  </si>
-  <si>
-    <t>no trans preload, coll dependency - water 129</t>
-  </si>
-  <si>
-    <t>4, limit 15, mult 1.5 seed 32628</t>
-  </si>
-  <si>
     <t>500,  27 - 2020202020191919</t>
   </si>
   <si>
-    <t>500,  27 - 2020202020202020</t>
+    <t>6000/6000/6000/2/0.00</t>
+  </si>
+  <si>
+    <t>5500/5500/5500/2/0.20</t>
+  </si>
+  <si>
+    <t>7000/7000/7000/2/0.00</t>
+  </si>
+  <si>
+    <t>8000/8000/8000/2/0.00</t>
+  </si>
+  <si>
+    <t>4000/4000/4000/2/0.00</t>
+  </si>
+  <si>
+    <t>6000/6000/6000/2/0.15</t>
+  </si>
+  <si>
+    <t>6000/6000/6000/2/0.20</t>
+  </si>
+  <si>
+    <t>LL regen settings (slst/neig/draw/prld/bwp)</t>
+  </si>
+  <si>
+    <t>5000/5000/5000/1/0.00</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 19805</t>
+  </si>
+  <si>
+    <t>only text preload, coll dependency - water 129</t>
+  </si>
+  <si>
+    <t>500, 239 - 2020202020202019</t>
+  </si>
+  <si>
+    <t>have not tried blue elev path</t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1005,56 +1008,59 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1383,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0D2D35-C0EE-42BD-9A8F-3836DBC519A6}">
   <dimension ref="B3:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1398,10 +1404,10 @@
     <col min="7" max="7" width="14" style="7" customWidth="1"/>
     <col min="8" max="8" width="5.33203125" style="7" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13" style="80" customWidth="1"/>
+    <col min="10" max="10" width="13" style="72" customWidth="1"/>
     <col min="11" max="11" width="28.109375" style="7" customWidth="1"/>
     <col min="12" max="12" width="13.109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" style="67" customWidth="1"/>
+    <col min="13" max="13" width="30.5546875" style="67" customWidth="1"/>
     <col min="14" max="14" width="39.109375" style="7" customWidth="1"/>
     <col min="15" max="15" width="33.88671875" style="7" customWidth="1"/>
     <col min="16" max="16" width="20.109375" style="67" customWidth="1"/>
@@ -1411,47 +1417,47 @@
   <sheetData>
     <row r="3" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="78"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="77" t="s">
+      <c r="F4" s="85"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="73" t="s">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="71" t="s">
+      <c r="S4" s="82" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="72"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>51</v>
@@ -1459,34 +1465,34 @@
       <c r="G5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="76"/>
+      <c r="H5" s="88"/>
       <c r="I5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M5" s="1" t="s">
         <v>108</v>
+      </c>
+      <c r="M5" s="71" t="s">
+        <v>165</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="72"/>
+        <v>119</v>
+      </c>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="83"/>
     </row>
     <row r="6" spans="2:19" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
@@ -1512,25 +1518,25 @@
         <v>98</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K6" s="38" t="s">
         <v>66</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M6" s="38" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P6" s="38" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>12</v>
@@ -1566,25 +1572,25 @@
         <v>104</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>66</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q7" s="10" t="s">
         <v>7</v>
@@ -1620,25 +1626,25 @@
         <v>116</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K8" s="39" t="s">
         <v>66</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P8" s="39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>8</v>
@@ -1674,25 +1680,25 @@
         <v>96</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>66</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="M9" s="40" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="Q9" s="13" t="s">
         <v>13</v>
@@ -1728,25 +1734,25 @@
         <v>104</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="L10" s="41" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="M10" s="41" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="O10" s="87" t="s">
-        <v>160</v>
+        <v>151</v>
+      </c>
+      <c r="O10" s="79" t="s">
+        <v>152</v>
       </c>
       <c r="P10" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q10" s="15" t="s">
         <v>14</v>
@@ -1820,25 +1826,25 @@
         <v>96</v>
       </c>
       <c r="J12" s="40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K12" s="40" t="s">
         <v>66</v>
       </c>
       <c r="L12" s="40" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="M12" s="40" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="P12" s="40" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="Q12" s="19" t="s">
         <v>16</v>
@@ -1912,25 +1918,25 @@
         <v>102</v>
       </c>
       <c r="J14" s="40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K14" s="40" t="s">
         <v>66</v>
       </c>
       <c r="L14" s="40" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="M14" s="40" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q14" s="19" t="s">
         <v>18</v>
@@ -2004,25 +2010,25 @@
         <v>104</v>
       </c>
       <c r="J16" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K16" s="41" t="s">
         <v>66</v>
       </c>
       <c r="L16" s="41" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="M16" s="41" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="N16" s="16" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="P16" s="41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q16" s="15" t="s">
         <v>20</v>
@@ -2131,19 +2137,19 @@
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="45">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K19" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="L19" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="M19" s="45" t="s">
         <v>166</v>
-      </c>
-      <c r="L19" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="M19" s="45" t="s">
-        <v>165</v>
       </c>
       <c r="N19" s="25" t="s">
         <v>167</v>
@@ -2151,7 +2157,9 @@
       <c r="O19" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="P19" s="45"/>
+      <c r="P19" s="45" t="s">
+        <v>170</v>
+      </c>
       <c r="Q19" s="24" t="s">
         <v>23</v>
       </c>
@@ -2300,25 +2308,25 @@
         <v>100</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K23" s="47" t="s">
         <v>66</v>
       </c>
       <c r="L23" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="P23" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="Q23" s="10" t="s">
         <v>27</v>
@@ -2353,26 +2361,26 @@
       <c r="I24" s="48">
         <v>80</v>
       </c>
-      <c r="J24" s="81" t="s">
-        <v>112</v>
+      <c r="J24" s="73" t="s">
+        <v>111</v>
       </c>
       <c r="K24" s="48" t="s">
         <v>66</v>
       </c>
       <c r="L24" s="48" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="O24" s="70" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q24" s="29" t="s">
         <v>28</v>
@@ -2405,7 +2413,7 @@
       </c>
       <c r="H25" s="25"/>
       <c r="I25" s="49"/>
-      <c r="J25" s="82"/>
+      <c r="J25" s="74"/>
       <c r="K25" s="49"/>
       <c r="L25" s="49"/>
       <c r="M25" s="45"/>
@@ -2481,7 +2489,7 @@
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="50"/>
-      <c r="J27" s="83"/>
+      <c r="J27" s="75"/>
       <c r="K27" s="69"/>
       <c r="L27" s="69"/>
       <c r="M27" s="46"/>
@@ -2522,25 +2530,25 @@
         <v>125</v>
       </c>
       <c r="J28" s="68" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K28" s="51" t="s">
         <v>66</v>
       </c>
       <c r="L28" s="51" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="M28" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="O28" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="N28" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="O28" s="33" t="s">
-        <v>138</v>
-      </c>
       <c r="P28" s="68" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q28" s="32" t="s">
         <v>32</v>
@@ -2573,7 +2581,7 @@
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="52"/>
-      <c r="J29" s="84"/>
+      <c r="J29" s="76"/>
       <c r="K29" s="52"/>
       <c r="L29" s="52"/>
       <c r="M29" s="44"/>
@@ -2649,7 +2657,7 @@
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="54"/>
-      <c r="J31" s="85"/>
+      <c r="J31" s="77"/>
       <c r="K31" s="54"/>
       <c r="L31" s="54"/>
       <c r="M31" s="42"/>
@@ -2689,26 +2697,26 @@
       <c r="I32" s="55">
         <v>110</v>
       </c>
-      <c r="J32" s="86" t="s">
-        <v>149</v>
+      <c r="J32" s="78" t="s">
+        <v>143</v>
       </c>
       <c r="K32" s="55" t="s">
         <v>66</v>
       </c>
       <c r="L32" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O32" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="O32" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="P32" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q32" s="37" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
rebuilt all vanilla c2pal levels with load list generation
</commit_message>
<xml_diff>
--- a/build files and notes/fluff/sheet w build methods info.xlsx
+++ b/build files and notes/fluff/sheet w build methods info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\fluff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91C5E40-7C8A-407B-BAB9-CE3B5E06CDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E7325-6B05-411D-AD53-80446FFE177B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView xWindow="18708" yWindow="5040" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="All level build notes" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="218">
   <si>
     <t>0A</t>
   </si>
@@ -375,18 +375,9 @@
     <t>Permaloaded list length</t>
   </si>
   <si>
-    <t>500, 116 - 2020202020202020</t>
-  </si>
-  <si>
-    <t>4, limit 20, mult 1.5 seed   863</t>
-  </si>
-  <si>
     <t>Iter count, best result</t>
   </si>
   <si>
-    <t>500,   1 - 2020202020201919</t>
-  </si>
-  <si>
     <t>01_uZ - 1</t>
   </si>
   <si>
@@ -399,60 +390,21 @@
     <t>no known issues</t>
   </si>
   <si>
-    <t>01_DZ</t>
-  </si>
-  <si>
-    <t>4, limit 20, mult 1.5 seed 22991</t>
-  </si>
-  <si>
-    <t>4, limit 20, mult 1.5 seed  5350</t>
-  </si>
-  <si>
-    <t>500,   1 - 2020191919181818</t>
-  </si>
-  <si>
-    <t>4, limit 20, mult 1.5 seed 26629</t>
-  </si>
-  <si>
-    <t>500,  11 - 2020191818181818</t>
-  </si>
-  <si>
     <t>01_aZ - 1</t>
   </si>
   <si>
     <t>0a_dZ - 2</t>
   </si>
   <si>
-    <t>4, limit 20, mult 1.5 seed 25579</t>
-  </si>
-  <si>
-    <t>500,   0 - 1818171616161616</t>
-  </si>
-  <si>
     <t>01_zZ - 1</t>
   </si>
   <si>
-    <t>4, limit 20, mult 1.5 seed 29472</t>
-  </si>
-  <si>
-    <t>500,   0 - 2019191818181818</t>
-  </si>
-  <si>
     <t>00_eZ - 1</t>
   </si>
   <si>
     <t>4, limit 15, mult 1.5 seed  1749</t>
   </si>
   <si>
-    <t>500,  19 - 1616161616151515</t>
-  </si>
-  <si>
-    <t>have not tried yellow elev path</t>
-  </si>
-  <si>
-    <t>have not tried secret route</t>
-  </si>
-  <si>
     <t>0a_hZ - 1</t>
   </si>
   <si>
@@ -462,18 +414,6 @@
     <t>500, 178 - 1717171716161616</t>
   </si>
   <si>
-    <t>have not tried   red plat path</t>
-  </si>
-  <si>
-    <t>general wrong 9-38</t>
-  </si>
-  <si>
-    <t>4, limit 19, mult 1.5 seed  7989</t>
-  </si>
-  <si>
-    <t>999, 200 - 2121202020202020</t>
-  </si>
-  <si>
     <t>a1_jZ - 1</t>
   </si>
   <si>
@@ -498,39 +438,18 @@
     <t>01_mZ - 2</t>
   </si>
   <si>
-    <t>4, limit 15, mult 1.5 seed  527</t>
-  </si>
-  <si>
-    <t>crashed until RatOC added into 26-04 deps</t>
-  </si>
-  <si>
     <t>01_pZ - 1</t>
   </si>
   <si>
-    <t>500,  27 - 2020202020191919</t>
-  </si>
-  <si>
     <t>6000/6000/6000/2/0.00</t>
   </si>
   <si>
-    <t>5500/5500/5500/2/0.20</t>
-  </si>
-  <si>
     <t>7000/7000/7000/2/0.00</t>
   </si>
   <si>
-    <t>8000/8000/8000/2/0.00</t>
-  </si>
-  <si>
     <t>4000/4000/4000/2/0.00</t>
   </si>
   <si>
-    <t>6000/6000/6000/2/0.15</t>
-  </si>
-  <si>
-    <t>6000/6000/6000/2/0.20</t>
-  </si>
-  <si>
     <t>LL regen settings (slst/neig/draw/prld/bwp)</t>
   </si>
   <si>
@@ -543,10 +462,232 @@
     <t>only text preload, coll dependency - water 129</t>
   </si>
   <si>
-    <t>500, 239 - 2020202020202019</t>
-  </si>
-  <si>
-    <t>have not tried blue elev path</t>
+    <t>01_wZ - 1</t>
+  </si>
+  <si>
+    <t>5000/5000/5000/2/0.00</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  5249</t>
+  </si>
+  <si>
+    <t>collision dependency - water 129</t>
+  </si>
+  <si>
+    <t>x4_xZ - 2</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 15238</t>
+  </si>
+  <si>
+    <t>500,  93 - 2120202020202020</t>
+  </si>
+  <si>
+    <t>5500/5500/5500/2/0.00</t>
+  </si>
+  <si>
+    <t>500, 192 - 2019191919191919</t>
+  </si>
+  <si>
+    <t>transitions lag (deliberate)</t>
+  </si>
+  <si>
+    <t>0a_iZ - 1</t>
+  </si>
+  <si>
+    <t>0a_qZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  5671</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  5508</t>
+  </si>
+  <si>
+    <t>permaloading A LOT, scuffed dependencies</t>
+  </si>
+  <si>
+    <t>400, 198 - 2120201919191919</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed   527</t>
+  </si>
+  <si>
+    <t>mult accidentally set really high</t>
+  </si>
+  <si>
+    <t>aa_CZ - 1</t>
+  </si>
+  <si>
+    <t>01_DZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 26770</t>
+  </si>
+  <si>
+    <t>500,  64 - 2121202020202020</t>
+  </si>
+  <si>
+    <t>aa_gZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 20767</t>
+  </si>
+  <si>
+    <t>500,  26 - 2019191919191919</t>
+  </si>
+  <si>
+    <t>01_tZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 11227</t>
+  </si>
+  <si>
+    <t>accidentally patched NSD with CrashEdit</t>
+  </si>
+  <si>
+    <t>500, 438 - 1919191919191919</t>
+  </si>
+  <si>
+    <t>01_yZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 16929</t>
+  </si>
+  <si>
+    <t>500,  55 - 2019191919191919</t>
+  </si>
+  <si>
+    <t>01_BZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 31242</t>
+  </si>
+  <si>
+    <t>500,  35 - 2020191919191919</t>
+  </si>
+  <si>
+    <t>500, 140 - 2091191919191919</t>
+  </si>
+  <si>
+    <t>500, 414 - 1919191818181818</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed   863</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  5350</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  7989</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 22991</t>
+  </si>
+  <si>
+    <t>500, 201 - 1818171717171717</t>
+  </si>
+  <si>
+    <t>500,  33 - 1616161616161616</t>
+  </si>
+  <si>
+    <t>500, 409 - 2120202020202020</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 26629</t>
+  </si>
+  <si>
+    <t>500, 298 - 2019191919181818</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 25579</t>
+  </si>
+  <si>
+    <t>500, 168 - 1616161616161616</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 29472</t>
+  </si>
+  <si>
+    <t>500,  52 - 1918181818181818</t>
+  </si>
+  <si>
+    <t>500,  17 - 2020201919191919</t>
+  </si>
+  <si>
+    <t>500,  62 - 2020202020191919</t>
+  </si>
+  <si>
+    <t>0a_lZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  4736</t>
+  </si>
+  <si>
+    <t>5k, 2077 - 2121202020202020</t>
+  </si>
+  <si>
+    <t>0a_AZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed  7743</t>
+  </si>
+  <si>
+    <t>permaloading A LOT,  coll dep - ice E3</t>
+  </si>
+  <si>
+    <t>500, 402 - 2020201919191918</t>
+  </si>
+  <si>
+    <t>alpine chase</t>
+  </si>
+  <si>
+    <t>secret -&gt; main small trans lag</t>
+  </si>
+  <si>
+    <t>bonus -&gt; path medium trans lag</t>
+  </si>
+  <si>
+    <t>01_nZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 23670</t>
+  </si>
+  <si>
+    <t>500, 397 - 2120202020202020</t>
+  </si>
+  <si>
+    <t>01_oZ - 1</t>
+  </si>
+  <si>
+    <t>crashed until BoudC was made permaloaded</t>
+  </si>
+  <si>
+    <t>crashed until RatOC was added into 26-4 deps</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 22303</t>
+  </si>
+  <si>
+    <t>500, 401 - 1919191919181818</t>
+  </si>
+  <si>
+    <t>main -&gt; secret small trans lag</t>
+  </si>
+  <si>
+    <t>only text preload, coll deps water 129, ice E3</t>
+  </si>
+  <si>
+    <t>coll dependency - ice E3</t>
+  </si>
+  <si>
+    <t>01_rZ - 1</t>
+  </si>
+  <si>
+    <t>4, limit 15, mult 1.5 seed 29958</t>
+  </si>
+  <si>
+    <t>500, 458 - 1818181818181818</t>
   </si>
 </sst>
 </file>
@@ -796,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1061,6 +1202,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1389,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0D2D35-C0EE-42BD-9A8F-3836DBC519A6}">
   <dimension ref="B3:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="L10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1473,22 +1626,22 @@
         <v>110</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>108</v>
       </c>
       <c r="M5" s="71" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="81"/>
       <c r="R5" s="81"/>
@@ -1518,25 +1671,25 @@
         <v>98</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K6" s="38" t="s">
         <v>66</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="M6" s="38" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="P6" s="38" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>12</v>
@@ -1572,7 +1725,7 @@
         <v>104</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>66</v>
@@ -1581,16 +1734,16 @@
         <v>109</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>120</v>
+        <v>203</v>
       </c>
       <c r="Q7" s="10" t="s">
         <v>7</v>
@@ -1626,25 +1779,25 @@
         <v>116</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K8" s="39" t="s">
         <v>66</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="P8" s="39" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>8</v>
@@ -1680,25 +1833,25 @@
         <v>96</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>66</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="M9" s="40" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="Q9" s="13" t="s">
         <v>13</v>
@@ -1737,22 +1890,22 @@
         <v>111</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>155</v>
+        <v>209</v>
       </c>
       <c r="L10" s="41" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="M10" s="41" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="O10" s="79" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="P10" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q10" s="15" t="s">
         <v>14</v>
@@ -1784,14 +1937,30 @@
         <v>57</v>
       </c>
       <c r="H11" s="18"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="42"/>
+      <c r="I11" s="42">
+        <v>95</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="L11" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="M11" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="P11" s="42" t="s">
+        <v>117</v>
+      </c>
       <c r="Q11" s="17" t="s">
         <v>15</v>
       </c>
@@ -1832,19 +2001,19 @@
         <v>66</v>
       </c>
       <c r="L12" s="40" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="M12" s="40" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="P12" s="40" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="Q12" s="19" t="s">
         <v>16</v>
@@ -1876,14 +2045,30 @@
         <v>59</v>
       </c>
       <c r="H13" s="21"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="43"/>
+      <c r="I13" s="43">
+        <v>121</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="M13" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="O13" s="90" t="s">
+        <v>148</v>
+      </c>
+      <c r="P13" s="43" t="s">
+        <v>117</v>
+      </c>
       <c r="Q13" s="20" t="s">
         <v>17</v>
       </c>
@@ -1924,19 +2109,19 @@
         <v>66</v>
       </c>
       <c r="L14" s="40" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="M14" s="40" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q14" s="19" t="s">
         <v>18</v>
@@ -1968,14 +2153,30 @@
         <v>60</v>
       </c>
       <c r="H15" s="23"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="44"/>
+      <c r="I15" s="44">
+        <v>107</v>
+      </c>
+      <c r="J15" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="M15" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="O15" s="92" t="s">
+        <v>196</v>
+      </c>
+      <c r="P15" s="44" t="s">
+        <v>117</v>
+      </c>
       <c r="Q15" s="22" t="s">
         <v>19</v>
       </c>
@@ -2016,19 +2217,19 @@
         <v>66</v>
       </c>
       <c r="L16" s="41" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="M16" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="N16" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="N16" s="16" t="s">
-        <v>154</v>
-      </c>
       <c r="O16" s="16" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="P16" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q16" s="15" t="s">
         <v>20</v>
@@ -2044,8 +2245,8 @@
       <c r="B17" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="63" t="s">
-        <v>44</v>
+      <c r="C17" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="D17" s="63">
         <v>17</v>
@@ -2060,19 +2261,35 @@
         <v>62</v>
       </c>
       <c r="H17" s="23"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="44"/>
+      <c r="I17" s="44">
+        <v>111</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="K17" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="M17" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="O17" s="92" t="s">
+        <v>206</v>
+      </c>
+      <c r="P17" s="44" t="s">
+        <v>212</v>
+      </c>
       <c r="Q17" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="63" t="s">
-        <v>44</v>
+      <c r="R17" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="S17" s="63">
         <v>17</v>
@@ -2082,8 +2299,8 @@
       <c r="B18" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="63" t="s">
-        <v>44</v>
+      <c r="C18" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="D18" s="63">
         <v>18</v>
@@ -2098,19 +2315,35 @@
         <v>63</v>
       </c>
       <c r="H18" s="23"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="44"/>
+      <c r="I18" s="44">
+        <v>99</v>
+      </c>
+      <c r="J18" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="L18" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="M18" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="O18" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="P18" s="44" t="s">
+        <v>117</v>
+      </c>
       <c r="Q18" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R18" s="63" t="s">
-        <v>44</v>
+      <c r="R18" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="S18" s="63">
         <v>18</v>
@@ -2143,22 +2376,22 @@
         <v>111</v>
       </c>
       <c r="K19" s="45" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="L19" s="45" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="M19" s="45" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="O19" s="25" t="s">
-        <v>169</v>
+        <v>140</v>
+      </c>
+      <c r="O19" s="89" t="s">
+        <v>148</v>
       </c>
       <c r="P19" s="45" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="Q19" s="24" t="s">
         <v>23</v>
@@ -2190,14 +2423,30 @@
         <v>64</v>
       </c>
       <c r="H20" s="21"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="43"/>
+      <c r="I20" s="43">
+        <v>120</v>
+      </c>
+      <c r="J20" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="L20" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="M20" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="O20" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="P20" s="43" t="s">
+        <v>117</v>
+      </c>
       <c r="Q20" s="26" t="s">
         <v>24</v>
       </c>
@@ -2212,8 +2461,8 @@
       <c r="B21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="63" t="s">
-        <v>44</v>
+      <c r="C21" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="D21" s="63" t="s">
         <v>6</v>
@@ -2228,19 +2477,35 @@
         <v>65</v>
       </c>
       <c r="H21" s="23"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="44"/>
+      <c r="I21" s="44">
+        <v>104</v>
+      </c>
+      <c r="J21" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="K21" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="L21" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="M21" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="O21" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="P21" s="44" t="s">
+        <v>117</v>
+      </c>
       <c r="Q21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="63" t="s">
-        <v>44</v>
+      <c r="R21" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="S21" s="63" t="s">
         <v>6</v>
@@ -2266,14 +2531,30 @@
         <v>68</v>
       </c>
       <c r="H22" s="28"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="46"/>
+      <c r="I22" s="46">
+        <v>121</v>
+      </c>
+      <c r="J22" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="L22" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="M22" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="N22" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="O22" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="P22" s="46" t="s">
+        <v>117</v>
+      </c>
       <c r="Q22" s="27" t="s">
         <v>26</v>
       </c>
@@ -2308,25 +2589,25 @@
         <v>100</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K23" s="47" t="s">
         <v>66</v>
       </c>
       <c r="L23" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="P23" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="Q23" s="10" t="s">
         <v>27</v>
@@ -2359,7 +2640,7 @@
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="48">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="J24" s="73" t="s">
         <v>111</v>
@@ -2368,19 +2649,19 @@
         <v>66</v>
       </c>
       <c r="L24" s="48" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="O24" s="70" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q24" s="29" t="s">
         <v>28</v>
@@ -2412,14 +2693,30 @@
         <v>73</v>
       </c>
       <c r="H25" s="25"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="45"/>
+      <c r="I25" s="49">
+        <v>103</v>
+      </c>
+      <c r="J25" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="K25" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="L25" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="M25" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="N25" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="O25" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="P25" s="45" t="s">
+        <v>151</v>
+      </c>
       <c r="Q25" s="30" t="s">
         <v>29</v>
       </c>
@@ -2450,14 +2747,30 @@
         <v>74</v>
       </c>
       <c r="H26" s="25"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="45"/>
+      <c r="I26" s="49">
+        <v>103</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="L26" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="M26" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="N26" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="O26" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="P26" s="45" t="s">
+        <v>117</v>
+      </c>
       <c r="Q26" s="30" t="s">
         <v>30</v>
       </c>
@@ -2488,14 +2801,30 @@
         <v>75</v>
       </c>
       <c r="H27" s="28"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="46"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="46"/>
+      <c r="I27" s="50">
+        <v>130</v>
+      </c>
+      <c r="J27" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="K27" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="L27" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="P27" s="46" t="s">
+        <v>117</v>
+      </c>
       <c r="Q27" s="31" t="s">
         <v>31</v>
       </c>
@@ -2530,25 +2859,25 @@
         <v>125</v>
       </c>
       <c r="J28" s="68" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K28" s="51" t="s">
         <v>66</v>
       </c>
       <c r="L28" s="51" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="M28" s="68" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="N28" s="33" t="s">
-        <v>132</v>
+        <v>190</v>
       </c>
       <c r="O28" s="33" t="s">
-        <v>133</v>
+        <v>191</v>
       </c>
       <c r="P28" s="68" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q28" s="32" t="s">
         <v>32</v>
@@ -2580,14 +2909,30 @@
         <v>77</v>
       </c>
       <c r="H29" s="23"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="44"/>
+      <c r="I29" s="52">
+        <v>108</v>
+      </c>
+      <c r="J29" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="K29" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="M29" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="N29" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="O29" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="P29" s="44" t="s">
+        <v>202</v>
+      </c>
       <c r="Q29" s="34" t="s">
         <v>33</v>
       </c>
@@ -2618,14 +2963,30 @@
         <v>78</v>
       </c>
       <c r="H30" s="28"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="46"/>
+      <c r="I30" s="53">
+        <v>133</v>
+      </c>
+      <c r="J30" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="K30" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="L30" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="M30" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="N30" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="O30" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="P30" s="46" t="s">
+        <v>117</v>
+      </c>
       <c r="Q30" s="35" t="s">
         <v>34</v>
       </c>
@@ -2656,14 +3017,30 @@
         <v>79</v>
       </c>
       <c r="H31" s="18"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="42"/>
+      <c r="I31" s="54">
+        <v>91</v>
+      </c>
+      <c r="J31" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="K31" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="L31" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="M31" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="N31" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="O31" s="91" t="s">
+        <v>163</v>
+      </c>
+      <c r="P31" s="42" t="s">
+        <v>117</v>
+      </c>
       <c r="Q31" s="36" t="s">
         <v>35</v>
       </c>
@@ -2698,25 +3075,25 @@
         <v>110</v>
       </c>
       <c r="J32" s="78" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="K32" s="55" t="s">
         <v>66</v>
       </c>
       <c r="L32" s="55" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q32" s="37" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
fixed a field in load list prop being incorrect sometimes, causing CE to show a bunch of errors when opening a level
</commit_message>
<xml_diff>
--- a/build files and notes/fluff/sheet w build methods info.xlsx
+++ b/build files and notes/fluff/sheet w build methods info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samo\OneDrive\Documents\C\C2export\build files and notes\fluff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/585e6af98e7a4d57/Documents/C/C2export/build files and notes/fluff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB6879B-E00F-4B5B-9975-1A3FFFE566E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{1E490236-A0EB-497A-A2CF-9F3A1114F1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
+    <workbookView xWindow="15384" yWindow="5040" windowWidth="7656" windowHeight="4200" xr2:uid="{C9098697-7CE0-4B37-8841-D91CE2D836A2}"/>
   </bookViews>
   <sheets>
     <sheet name="All level build notes" sheetId="3" r:id="rId1"/>
@@ -699,7 +699,7 @@
     <t>lags before first checkpoint</t>
   </si>
   <si>
-    <t>smashers wrong dep list (missing CdSeV</t>
+    <t>smashers wrong dep list (missing CdSeV)</t>
   </si>
 </sst>
 </file>
@@ -1554,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0D2D35-C0EE-42BD-9A8F-3836DBC519A6}">
   <dimension ref="B3:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>